<commit_message>
added overall stats, adams
</commit_message>
<xml_diff>
--- a/Yearly Reports/2018/Adams/Adams Report.xlsx
+++ b/Yearly Reports/2018/Adams/Adams Report.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FitzFishing\Yearly Reports\2018\Adams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FCB1E8-8EBE-484D-BCF1-847FB986F44E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45499018-BBAB-4A40-9BC1-F9B704146902}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="2" r:id="rId1"/>
     <sheet name="2018" sheetId="1" r:id="rId2"/>
+    <sheet name="Overall Stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
   <si>
     <t>Lake/Pond</t>
   </si>
@@ -182,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +241,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -302,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,9 +353,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -364,6 +377,2107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TOTAL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> SPECIES CAUGHT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="27000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Overall Stats'!$A$2:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Rainbow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Brown</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bluegill</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wiper</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brook</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Stats'!$A$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2DCD-42D5-AAA0-FAE76B0F9A2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="84"/>
+        <c:gapDepth val="53"/>
+        <c:shape val="box"/>
+        <c:axId val="1489081503"/>
+        <c:axId val="1688145439"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1489081503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1688145439"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1688145439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1489081503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PERCENT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> SPECIES CAUGHT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Overall Stats'!$A$5:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Rainbow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Brown</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bluegill</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wiper</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brook</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Stats'!$A$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>79.586563307493535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2351421188630489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.144702842377262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77519379844961245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2583979328165375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5FC-4EC7-A6CF-ED7FB4C861F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="291">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:tint val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="27000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="0" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FB50E4-9B12-4C09-944F-8273A38ECC11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A129990-494C-402B-BB16-EEA274E01A4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -629,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ED1804-F28B-46A1-9F98-8A4AF52A987D}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,13 +2756,13 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -657,7 +2771,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -671,15 +2785,14 @@
       <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -699,13 +2812,10 @@
         <v>28</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -720,7 +2830,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="8">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G4" s="8">
         <v>22</v>
@@ -729,13 +2839,10 @@
         <v>38</v>
       </c>
       <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -755,9 +2862,8 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -781,13 +2887,10 @@
         <v>28</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -803,10 +2906,10 @@
       </c>
       <c r="F7" s="8">
         <f>SUM(F4/$D$25*100)</f>
-        <v>72.995780590717303</v>
+        <v>73.417721518987349</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" ref="G7:J7" si="0">SUM(G4/$D$25*100)</f>
+        <f t="shared" ref="G7:I7" si="0">SUM(G4/$D$25*100)</f>
         <v>9.2827004219409286</v>
       </c>
       <c r="H7" s="8">
@@ -815,14 +2918,10 @@
       </c>
       <c r="I7" s="8">
         <f t="shared" si="0"/>
-        <v>0.42194092827004215</v>
-      </c>
-      <c r="J7" s="8">
-        <f t="shared" si="0"/>
         <v>1.2658227848101267</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -837,7 +2936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -852,7 +2951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -867,7 +2966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -882,7 +2981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -897,7 +2996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -912,7 +3011,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
@@ -927,7 +3026,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
@@ -942,7 +3041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
@@ -1106,8 +3205,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1566,4 +3665,153 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1CA989-3A01-4014-AE07-8387268A40B0}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <f>SUM('2017'!F4+'2018'!I4)</f>
+        <v>308</v>
+      </c>
+      <c r="B3" s="8">
+        <f>SUM('2017'!G4+'2018'!J4)</f>
+        <v>28</v>
+      </c>
+      <c r="C3" s="8">
+        <f>SUM('2017'!H4+'2018'!L4)</f>
+        <v>47</v>
+      </c>
+      <c r="D3" s="8">
+        <f>SUM('2017'!I4)</f>
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <f>SUM('2018'!K4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <f>SUM(A3/$B$8*100)</f>
+        <v>79.586563307493535</v>
+      </c>
+      <c r="B6" s="8">
+        <f t="shared" ref="B6:E6" si="0">SUM(B3/$B$8*100)</f>
+        <v>7.2351421188630489</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
+        <v>12.144702842377262</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.77519379844961245</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2583979328165375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="18">
+        <f>SUM('2017'!D25+'2018'!G20)</f>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="18">
+        <f>SUM('2017'!D26+'2018'!G21)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="21">
+        <f>SUM(B8/B9)</f>
+        <v>10.184210526315789</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated all lake files
</commit_message>
<xml_diff>
--- a/Yearly Reports/2018/Adams/Adams Report.xlsx
+++ b/Yearly Reports/2018/Adams/Adams Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\Fishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40E47B6-1437-4780-8AB0-C936155B97AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DB8FAA-5A6F-4C74-9FC7-A1D7E0FF440C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="53">
   <si>
     <t>Lake/Pond</t>
   </si>
@@ -177,13 +177,22 @@
   </si>
   <si>
     <t>Fishing Report 2017 Adams</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>RATING</t>
+  </si>
+  <si>
+    <t>Fair</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +259,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1D00F2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -310,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +372,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,8 +387,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -371,6 +403,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF1D00F2"/>
+      <color rgb="FF2805BB"/>
+      <color rgb="FF17036D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2437,13 +2476,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2471,15 +2510,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2771,10 +2810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ED1804-F28B-46A1-9F98-8A4AF52A987D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2803,22 +2842,22 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
@@ -2884,12 +2923,12 @@
       <c r="E5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -2932,20 +2971,20 @@
       <c r="E7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="18">
         <f>SUM(F4/$D$25*100)</f>
         <v>9.2827004219409286</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="18">
         <f>SUM(G4/$D$25*100)</f>
         <v>16.033755274261605</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="18">
         <f>SUM(H4/$D$25*100)</f>
         <v>73.417721518987349</v>
       </c>
-      <c r="I7" s="22">
-        <f t="shared" ref="G7:I7" si="0">SUM(I4/$D$25*100)</f>
+      <c r="I7" s="18">
+        <f t="shared" ref="I7" si="0">SUM(I4/$D$25*100)</f>
         <v>1.2658227848101267</v>
       </c>
     </row>
@@ -3228,6 +3267,14 @@
       <c r="D27" s="12">
         <f>AVERAGE(D4:D24)</f>
         <v>11.285714285714286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3237,15 +3284,16 @@
     <mergeCell ref="F5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3276,23 +3324,23 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -3373,12 +3421,12 @@
       <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -3427,19 +3475,19 @@
       <c r="H7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="18">
         <f>SUM(I4/$G$20*100)</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="18">
         <f>SUM(J4/$G$20*100)</f>
         <v>4</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="18">
         <f>SUM(K4/$G$20*100)</f>
         <v>6</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="18">
         <f>SUM(L4/$G$20*100)</f>
         <v>89.333333333333329</v>
       </c>
@@ -3684,6 +3732,14 @@
       <c r="G22" s="12">
         <f>SUM(G20/G21)</f>
         <v>9.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3698,10 +3754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1CA989-3A01-4014-AE07-8387268A40B0}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,13 +3770,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -3762,13 +3818,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -3788,23 +3844,23 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="18">
         <f>SUM(A3/$B$8*100)</f>
         <v>0.2583979328165375</v>
       </c>
-      <c r="B6" s="22">
-        <f t="shared" ref="B6:E6" si="0">SUM(B3/$B$8*100)</f>
+      <c r="B6" s="18">
+        <f t="shared" ref="B6:C6" si="0">SUM(B3/$B$8*100)</f>
         <v>7.2351421188630489</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="18">
         <f t="shared" si="0"/>
         <v>12.144702842377262</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="18">
         <f>SUM(D3/$B$8*100)</f>
         <v>79.586563307493535</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="18">
         <f>SUM(E3/$B$8*100)</f>
         <v>0.77519379844961245</v>
       </c>
@@ -3834,6 +3890,14 @@
       <c r="B10" s="17">
         <f>SUM(B8/B9)</f>
         <v>10.184210526315789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>